<commit_message>
Added solving linear equations
</commit_message>
<xml_diff>
--- a/projectile_motion_data.xlsx
+++ b/projectile_motion_data.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>x_position</t>
+          <t>x position</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>y_position</t>
+          <t>y position</t>
         </is>
       </c>
     </row>

</xml_diff>